<commit_message>
Mise à jour sprint 6
</commit_message>
<xml_diff>
--- a/Documents/Scrum/Sprint_backlog.xlsx
+++ b/Documents/Scrum/Sprint_backlog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\angel\Documents\GitHub\WavContact\Documents\Scrum\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09FB1C74-446A-4B0E-8C12-ECD879ABDCBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4C88DAC-1467-4D8B-81F4-73580ADFC079}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="4" activeTab="6" xr2:uid="{BBA08FA1-3D47-4FFE-8A0F-E0679BA05BA2}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="2" activeTab="2" xr2:uid="{BBA08FA1-3D47-4FFE-8A0F-E0679BA05BA2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint_0." sheetId="4" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="Sprint_4." sheetId="7" r:id="rId5"/>
     <sheet name="Sprint_5." sheetId="5" r:id="rId6"/>
     <sheet name="Sprint_6." sheetId="6" r:id="rId7"/>
+    <sheet name="Sprint_7." sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="239">
   <si>
     <t>STORY</t>
   </si>
@@ -701,9 +702,6 @@
   </si>
   <si>
     <t>Insérer dans table réservation ajouter id matériel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Manuel utilisateur </t>
   </si>
   <si>
     <t>Manuel d'installation</t>
@@ -2022,6 +2020,334 @@
   </si>
   <si>
     <t>Faire le POST et DELETE pour la fenêtre "stock matériel"</t>
+  </si>
+  <si>
+    <t>Documentation
+jeux de tests</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Documenter le test login correct </t>
+  </si>
+  <si>
+    <t>Documenter le test login incorrect</t>
+  </si>
+  <si>
+    <t>Documenter le test get user</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Documenter le create user </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="9" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Client</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> : Expliquer en détail pour les utilisateurs la view pour le chat </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="9" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Client</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> : Expliquer en détail pour les utilisateurs la view de la page principale</t>
+    </r>
+  </si>
+  <si>
+    <t>Manuel utilisateur  et membre
+WavCom</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Membre</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Expliquer en détail pour les membres la view pour le chat </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Membre</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Expliquer en détail pour les membres la view pour la gestion de projet  </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Membre</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: Expliquer en détail pour les membres la view pour la gestion de stock </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Membre</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Expliquer en détail pour les membres la view pour les projets </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Membre</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Expliquer en détail pour les membres la view page principale</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Commun</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> : Expliquer en détail pour les utilisateurs et membres la view du login</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Commun</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> : Expliquer en détail pour les utilisateurs et membres la view du mot de passe oublié</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Commun</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> : Expliquer en détail pour les utilisateurs et membres la view des paramètres </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Commun</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> : Expliquer en détail pour les utilisateurs et membres la view des projets</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -2507,7 +2833,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="106">
+  <cellXfs count="108">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -2649,7 +2975,6 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2712,12 +3037,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2769,7 +3094,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3123,11 +3457,11 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="58" x14ac:dyDescent="0.35">
-      <c r="A2" s="88" t="s">
+      <c r="A2" s="87" t="s">
         <v>20</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -3137,7 +3471,7 @@
       <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" s="89"/>
+      <c r="A3" s="88"/>
       <c r="B3" s="2" t="s">
         <v>14</v>
       </c>
@@ -3149,7 +3483,7 @@
       <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" s="89"/>
+      <c r="A4" s="88"/>
       <c r="B4" s="2" t="s">
         <v>15</v>
       </c>
@@ -3161,7 +3495,7 @@
       <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" s="89"/>
+      <c r="A5" s="88"/>
       <c r="B5" s="2" t="s">
         <v>16</v>
       </c>
@@ -3173,7 +3507,7 @@
       <c r="F5" s="1"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A6" s="89"/>
+      <c r="A6" s="88"/>
       <c r="B6" s="2" t="s">
         <v>17</v>
       </c>
@@ -3185,7 +3519,7 @@
       <c r="F6" s="1"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A7" s="89"/>
+      <c r="A7" s="88"/>
       <c r="B7" s="2" t="s">
         <v>18</v>
       </c>
@@ -3197,7 +3531,7 @@
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A8" s="90"/>
+      <c r="A8" s="89"/>
       <c r="B8" s="2" t="s">
         <v>19</v>
       </c>
@@ -3209,15 +3543,15 @@
       <c r="F8" s="1"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A9" s="68"/>
-      <c r="B9" s="69"/>
-      <c r="C9" s="69"/>
-      <c r="D9" s="69"/>
-      <c r="E9" s="70"/>
+      <c r="A9" s="67"/>
+      <c r="B9" s="68"/>
+      <c r="C9" s="68"/>
+      <c r="D9" s="68"/>
+      <c r="E9" s="69"/>
       <c r="F9" s="1"/>
     </row>
     <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="91" t="s">
+      <c r="A10" s="90" t="s">
         <v>27</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -3230,7 +3564,7 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A11" s="92"/>
+      <c r="A11" s="91"/>
       <c r="B11" s="2" t="s">
         <v>22</v>
       </c>
@@ -3241,7 +3575,7 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A12" s="92"/>
+      <c r="A12" s="91"/>
       <c r="B12" s="2" t="s">
         <v>23</v>
       </c>
@@ -3253,7 +3587,7 @@
       <c r="H12" s="1"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A13" s="92"/>
+      <c r="A13" s="91"/>
       <c r="B13" s="2" t="s">
         <v>75</v>
       </c>
@@ -3265,7 +3599,7 @@
       <c r="H13" s="1"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A14" s="92"/>
+      <c r="A14" s="91"/>
       <c r="B14" s="2" t="s">
         <v>24</v>
       </c>
@@ -3276,7 +3610,7 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A15" s="92"/>
+      <c r="A15" s="91"/>
       <c r="B15" s="2" t="s">
         <v>25</v>
       </c>
@@ -3287,7 +3621,7 @@
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A16" s="92"/>
+      <c r="A16" s="91"/>
       <c r="B16" s="2" t="s">
         <v>26</v>
       </c>
@@ -3298,31 +3632,31 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17" s="92"/>
-      <c r="B17" s="58" t="s">
+      <c r="A17" s="91"/>
+      <c r="B17" s="57" t="s">
+        <v>186</v>
+      </c>
+      <c r="C17" s="57"/>
+      <c r="D17" s="57"/>
+      <c r="E17" s="70" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18" s="91"/>
+      <c r="B18" s="57" t="s">
         <v>187</v>
       </c>
-      <c r="C17" s="58"/>
-      <c r="D17" s="58"/>
-      <c r="E17" s="71" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A18" s="92"/>
-      <c r="B18" s="58" t="s">
+      <c r="C18" s="57"/>
+      <c r="D18" s="57"/>
+      <c r="E18" s="70" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="92"/>
+      <c r="B19" s="6" t="s">
         <v>188</v>
-      </c>
-      <c r="C18" s="58"/>
-      <c r="D18" s="58"/>
-      <c r="E18" s="71" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="93"/>
-      <c r="B19" s="6" t="s">
-        <v>189</v>
       </c>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
@@ -3373,7 +3707,7 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A2" s="94" t="s">
+      <c r="A2" s="93" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="17" t="s">
@@ -3387,9 +3721,9 @@
       <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" s="95"/>
+      <c r="A3" s="94"/>
       <c r="B3" s="17" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -3399,7 +3733,7 @@
       <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A4" s="95"/>
+      <c r="A4" s="94"/>
       <c r="B4" s="17" t="s">
         <v>9</v>
       </c>
@@ -3411,7 +3745,7 @@
       <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" s="95"/>
+      <c r="A5" s="94"/>
       <c r="B5" s="2" t="s">
         <v>10</v>
       </c>
@@ -3422,9 +3756,9 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" s="95"/>
+      <c r="A6" s="94"/>
       <c r="B6" s="17" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
@@ -3434,7 +3768,7 @@
       <c r="H6" s="1"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A7" s="95"/>
+      <c r="A7" s="94"/>
       <c r="B7" s="2" t="s">
         <v>6</v>
       </c>
@@ -3445,9 +3779,9 @@
       </c>
     </row>
     <row r="8" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="95"/>
+      <c r="A8" s="94"/>
       <c r="B8" s="17" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
@@ -3456,7 +3790,7 @@
       </c>
     </row>
     <row r="9" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A9" s="95"/>
+      <c r="A9" s="94"/>
       <c r="B9" s="17" t="s">
         <v>11</v>
       </c>
@@ -3467,7 +3801,7 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A10" s="95"/>
+      <c r="A10" s="94"/>
       <c r="B10" s="2" t="s">
         <v>7</v>
       </c>
@@ -3478,9 +3812,9 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A11" s="95"/>
+      <c r="A11" s="94"/>
       <c r="B11" s="17" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
@@ -3489,9 +3823,9 @@
       </c>
     </row>
     <row r="12" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A12" s="95"/>
+      <c r="A12" s="94"/>
       <c r="B12" s="17" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
@@ -3500,9 +3834,9 @@
       </c>
     </row>
     <row r="13" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A13" s="96"/>
+      <c r="A13" s="95"/>
       <c r="B13" s="17" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
@@ -3511,22 +3845,22 @@
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A14" s="76"/>
-      <c r="B14" s="77"/>
-      <c r="C14" s="77"/>
-      <c r="D14" s="77"/>
-      <c r="E14" s="78"/>
+      <c r="A14" s="75"/>
+      <c r="B14" s="76"/>
+      <c r="C14" s="76"/>
+      <c r="D14" s="76"/>
+      <c r="E14" s="77"/>
     </row>
     <row r="15" spans="1:8" ht="35.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="80" t="s">
+      <c r="A15" s="79" t="s">
+        <v>215</v>
+      </c>
+      <c r="B15" s="80" t="s">
         <v>216</v>
-      </c>
-      <c r="B15" s="81" t="s">
-        <v>217</v>
       </c>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
-      <c r="E15" s="79" t="s">
+      <c r="E15" s="78" t="s">
         <v>12</v>
       </c>
     </row>
@@ -3544,7 +3878,7 @@
   <sheetPr codeName="Feuil2"/>
   <dimension ref="A1:F48"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A17" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="82" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
@@ -3573,10 +3907,10 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="29.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="91" t="s">
+      <c r="A2" s="90" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="65" t="s">
+      <c r="B2" s="64" t="s">
         <v>112</v>
       </c>
       <c r="C2" s="25"/>
@@ -3587,8 +3921,8 @@
       <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:6" ht="29.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="92"/>
-      <c r="B3" s="65" t="s">
+      <c r="A3" s="91"/>
+      <c r="B3" s="64" t="s">
         <v>106</v>
       </c>
       <c r="C3" s="25"/>
@@ -3599,8 +3933,8 @@
       <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:6" ht="29.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="92"/>
-      <c r="B4" s="65" t="s">
+      <c r="A4" s="91"/>
+      <c r="B4" s="64" t="s">
         <v>120</v>
       </c>
       <c r="C4" s="25"/>
@@ -3611,8 +3945,8 @@
       <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:6" ht="29.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="92"/>
-      <c r="B5" s="65" t="s">
+      <c r="A5" s="91"/>
+      <c r="B5" s="64" t="s">
         <v>107</v>
       </c>
       <c r="C5" s="25"/>
@@ -3623,8 +3957,8 @@
       <c r="F5" s="1"/>
     </row>
     <row r="6" spans="1:6" ht="29.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="92"/>
-      <c r="B6" s="65" t="s">
+      <c r="A6" s="91"/>
+      <c r="B6" s="64" t="s">
         <v>121</v>
       </c>
       <c r="C6" s="25"/>
@@ -3635,8 +3969,8 @@
       <c r="F6" s="1"/>
     </row>
     <row r="7" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A7" s="92"/>
-      <c r="B7" s="65" t="s">
+      <c r="A7" s="91"/>
+      <c r="B7" s="64" t="s">
         <v>109</v>
       </c>
       <c r="C7" s="25"/>
@@ -3647,9 +3981,9 @@
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6" ht="29.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="92"/>
-      <c r="B8" s="65" t="s">
-        <v>193</v>
+      <c r="A8" s="91"/>
+      <c r="B8" s="64" t="s">
+        <v>192</v>
       </c>
       <c r="C8" s="25"/>
       <c r="D8" s="2"/>
@@ -3659,8 +3993,8 @@
       <c r="F8" s="1"/>
     </row>
     <row r="9" spans="1:6" ht="29.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="92"/>
-      <c r="B9" s="65" t="s">
+      <c r="A9" s="91"/>
+      <c r="B9" s="64" t="s">
         <v>108</v>
       </c>
       <c r="C9" s="25"/>
@@ -3671,8 +4005,8 @@
       <c r="F9" s="1"/>
     </row>
     <row r="10" spans="1:6" ht="29.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="92"/>
-      <c r="B10" s="65" t="s">
+      <c r="A10" s="91"/>
+      <c r="B10" s="64" t="s">
         <v>110</v>
       </c>
       <c r="C10" s="25"/>
@@ -3683,9 +4017,9 @@
       <c r="F10" s="1"/>
     </row>
     <row r="11" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A11" s="92"/>
-      <c r="B11" s="65" t="s">
-        <v>194</v>
+      <c r="A11" s="91"/>
+      <c r="B11" s="64" t="s">
+        <v>193</v>
       </c>
       <c r="C11" s="25"/>
       <c r="D11" s="2"/>
@@ -3695,9 +4029,9 @@
       <c r="F11" s="1"/>
     </row>
     <row r="12" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="92"/>
-      <c r="B12" s="65" t="s">
-        <v>195</v>
+      <c r="A12" s="91"/>
+      <c r="B12" s="64" t="s">
+        <v>194</v>
       </c>
       <c r="C12" s="25"/>
       <c r="D12" s="2"/>
@@ -3707,8 +4041,8 @@
       <c r="F12" s="1"/>
     </row>
     <row r="13" spans="1:6" ht="29.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="92"/>
-      <c r="B13" s="65" t="s">
+      <c r="A13" s="91"/>
+      <c r="B13" s="64" t="s">
         <v>111</v>
       </c>
       <c r="C13" s="25"/>
@@ -3719,9 +4053,9 @@
       <c r="F13" s="1"/>
     </row>
     <row r="14" spans="1:6" ht="29.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="92"/>
-      <c r="B14" s="65" t="s">
-        <v>196</v>
+      <c r="A14" s="91"/>
+      <c r="B14" s="64" t="s">
+        <v>195</v>
       </c>
       <c r="C14" s="25"/>
       <c r="D14" s="2"/>
@@ -3731,8 +4065,8 @@
       <c r="F14" s="1"/>
     </row>
     <row r="15" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="92"/>
-      <c r="B15" s="65" t="s">
+      <c r="A15" s="91"/>
+      <c r="B15" s="64" t="s">
         <v>113</v>
       </c>
       <c r="C15" s="25"/>
@@ -3743,8 +4077,8 @@
       <c r="F15" s="1"/>
     </row>
     <row r="16" spans="1:6" ht="29.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="92"/>
-      <c r="B16" s="65" t="s">
+      <c r="A16" s="91"/>
+      <c r="B16" s="64" t="s">
         <v>114</v>
       </c>
       <c r="C16" s="25"/>
@@ -3755,8 +4089,8 @@
       <c r="F16" s="1"/>
     </row>
     <row r="17" spans="1:6" ht="29.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="92"/>
-      <c r="B17" s="65" t="s">
+      <c r="A17" s="91"/>
+      <c r="B17" s="64" t="s">
         <v>117</v>
       </c>
       <c r="C17" s="25"/>
@@ -3767,8 +4101,8 @@
       <c r="F17" s="1"/>
     </row>
     <row r="18" spans="1:6" ht="29.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="92"/>
-      <c r="B18" s="65" t="s">
+      <c r="A18" s="91"/>
+      <c r="B18" s="64" t="s">
         <v>116</v>
       </c>
       <c r="C18" s="25"/>
@@ -3779,8 +4113,8 @@
       <c r="F18" s="1"/>
     </row>
     <row r="19" spans="1:6" ht="29.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="92"/>
-      <c r="B19" s="65" t="s">
+      <c r="A19" s="91"/>
+      <c r="B19" s="64" t="s">
         <v>115</v>
       </c>
       <c r="C19" s="25"/>
@@ -3791,8 +4125,8 @@
       <c r="F19" s="1"/>
     </row>
     <row r="20" spans="1:6" ht="29.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="92"/>
-      <c r="B20" s="65" t="s">
+      <c r="A20" s="91"/>
+      <c r="B20" s="64" t="s">
         <v>118</v>
       </c>
       <c r="C20" s="25"/>
@@ -3803,8 +4137,8 @@
       <c r="F20" s="1"/>
     </row>
     <row r="21" spans="1:6" ht="29.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="97"/>
-      <c r="B21" s="65" t="s">
+      <c r="A21" s="96"/>
+      <c r="B21" s="64" t="s">
         <v>119</v>
       </c>
       <c r="C21" s="25"/>
@@ -3823,256 +4157,256 @@
       <c r="F22" s="1"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A23" s="98" t="s">
+      <c r="A23" s="97" t="s">
         <v>29</v>
       </c>
       <c r="B23" s="38" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C23" s="25"/>
       <c r="D23" s="2"/>
       <c r="E23" s="18" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F23" s="1"/>
     </row>
     <row r="24" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A24" s="99"/>
+      <c r="A24" s="98"/>
       <c r="B24" s="17" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C24" s="25"/>
       <c r="D24" s="2"/>
       <c r="E24" s="18" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F24" s="1"/>
     </row>
     <row r="25" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A25" s="99"/>
+      <c r="A25" s="98"/>
       <c r="B25" s="17" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C25" s="25"/>
       <c r="D25" s="2"/>
       <c r="E25" s="18" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F25" s="1"/>
     </row>
     <row r="26" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A26" s="99"/>
+      <c r="A26" s="98"/>
       <c r="B26" s="17" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C26" s="25"/>
       <c r="D26" s="2"/>
       <c r="E26" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="F26" s="1"/>
+    </row>
+    <row r="27" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A27" s="98"/>
+      <c r="B27" s="65" t="s">
         <v>168</v>
-      </c>
-      <c r="F26" s="1"/>
-    </row>
-    <row r="27" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A27" s="99"/>
-      <c r="B27" s="66" t="s">
-        <v>169</v>
       </c>
       <c r="C27" s="25"/>
       <c r="D27" s="2"/>
       <c r="E27" s="18" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F27" s="1"/>
     </row>
     <row r="28" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A28" s="99"/>
+      <c r="A28" s="98"/>
       <c r="B28" s="17" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C28" s="25"/>
       <c r="D28" s="2"/>
       <c r="E28" s="18" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F28" s="1"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A29" s="99"/>
+      <c r="A29" s="98"/>
       <c r="B29" s="17" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C29" s="25"/>
       <c r="D29" s="2"/>
       <c r="E29" s="18" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F29" s="1"/>
     </row>
     <row r="30" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A30" s="99"/>
+      <c r="A30" s="98"/>
       <c r="B30" s="17" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C30" s="25"/>
       <c r="D30" s="2"/>
       <c r="E30" s="18" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F30" s="1"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A31" s="99"/>
+      <c r="A31" s="98"/>
       <c r="B31" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C31" s="25"/>
       <c r="D31" s="2"/>
       <c r="E31" s="18" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F31" s="1"/>
     </row>
     <row r="32" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A32" s="99"/>
+      <c r="A32" s="98"/>
       <c r="B32" s="17" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C32" s="25"/>
       <c r="D32" s="2"/>
       <c r="E32" s="18" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F32" s="1"/>
     </row>
     <row r="33" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A33" s="99"/>
-      <c r="B33" s="66" t="s">
-        <v>176</v>
+      <c r="A33" s="98"/>
+      <c r="B33" s="65" t="s">
+        <v>175</v>
       </c>
       <c r="C33" s="25"/>
       <c r="D33" s="2"/>
       <c r="E33" s="18" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F33" s="1"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A34" s="99"/>
+      <c r="A34" s="98"/>
       <c r="B34" s="38" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C34" s="25"/>
       <c r="D34" s="2"/>
       <c r="E34" s="18" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F34" s="1"/>
     </row>
     <row r="35" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A35" s="99"/>
-      <c r="B35" s="67" t="s">
-        <v>177</v>
+      <c r="A35" s="98"/>
+      <c r="B35" s="66" t="s">
+        <v>176</v>
       </c>
       <c r="C35" s="25"/>
       <c r="D35" s="2"/>
       <c r="E35" s="18" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F35" s="1"/>
     </row>
     <row r="36" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A36" s="99"/>
-      <c r="B36" s="66" t="s">
-        <v>178</v>
+      <c r="A36" s="98"/>
+      <c r="B36" s="65" t="s">
+        <v>177</v>
       </c>
       <c r="C36" s="25"/>
       <c r="D36" s="2"/>
       <c r="E36" s="18" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F36" s="1"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A37" s="99"/>
+      <c r="A37" s="98"/>
       <c r="B37" s="41" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C37" s="25"/>
       <c r="D37" s="2"/>
       <c r="E37" s="18" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F37" s="1"/>
     </row>
     <row r="38" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A38" s="99"/>
-      <c r="B38" s="66" t="s">
-        <v>179</v>
+      <c r="A38" s="98"/>
+      <c r="B38" s="65" t="s">
+        <v>178</v>
       </c>
       <c r="C38" s="25"/>
       <c r="D38" s="2"/>
       <c r="E38" s="18" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F38" s="1"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A39" s="99"/>
+      <c r="A39" s="98"/>
       <c r="B39" s="38" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C39" s="25"/>
       <c r="D39" s="2"/>
       <c r="E39" s="18" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F39" s="1"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A40" s="99"/>
+      <c r="A40" s="98"/>
       <c r="B40" s="38" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C40" s="25"/>
       <c r="D40" s="2"/>
       <c r="E40" s="18" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F40" s="1"/>
     </row>
     <row r="41" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A41" s="99"/>
-      <c r="B41" s="66" t="s">
-        <v>181</v>
+      <c r="A41" s="98"/>
+      <c r="B41" s="65" t="s">
+        <v>180</v>
       </c>
       <c r="C41" s="25"/>
       <c r="D41" s="2"/>
       <c r="E41" s="18" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F41" s="1"/>
     </row>
     <row r="42" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A42" s="99"/>
-      <c r="B42" s="66" t="s">
-        <v>180</v>
+      <c r="A42" s="98"/>
+      <c r="B42" s="65" t="s">
+        <v>179</v>
       </c>
       <c r="C42" s="25"/>
       <c r="D42" s="2"/>
       <c r="E42" s="18" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F42" s="1"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A43" s="100"/>
+      <c r="A43" s="99"/>
       <c r="B43" s="38" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C43" s="25"/>
       <c r="D43" s="2"/>
       <c r="E43" s="18" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F43" s="1"/>
     </row>
@@ -4085,7 +4419,7 @@
       <c r="F44" s="1"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A45" s="98" t="s">
+      <c r="A45" s="97" t="s">
         <v>76</v>
       </c>
       <c r="B45" s="2" t="s">
@@ -4099,11 +4433,11 @@
       <c r="F45" s="1"/>
     </row>
     <row r="46" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A46" s="101"/>
+      <c r="A46" s="100"/>
       <c r="B46" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C46" s="73"/>
+      <c r="C46" s="72"/>
       <c r="D46" s="6"/>
       <c r="E46" s="43" t="s">
         <v>12</v>
@@ -4140,7 +4474,7 @@
   <sheetPr codeName="Feuil3"/>
   <dimension ref="A1:H48"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="B26" sqref="B26:B36"/>
     </sheetView>
   </sheetViews>
@@ -4169,7 +4503,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="91" t="s">
+      <c r="A2" s="90" t="s">
         <v>73</v>
       </c>
       <c r="B2" s="38" t="s">
@@ -4183,9 +4517,9 @@
       <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="99"/>
+      <c r="A3" s="98"/>
       <c r="B3" s="38" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C3" s="39"/>
       <c r="D3" s="40"/>
@@ -4195,7 +4529,7 @@
       <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="99"/>
+      <c r="A4" s="98"/>
       <c r="B4" s="38" t="s">
         <v>52</v>
       </c>
@@ -4207,7 +4541,7 @@
       <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="99"/>
+      <c r="A5" s="98"/>
       <c r="B5" s="2" t="s">
         <v>51</v>
       </c>
@@ -4219,7 +4553,7 @@
       <c r="F5" s="1"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="99"/>
+      <c r="A6" s="98"/>
       <c r="B6" s="2" t="s">
         <v>53</v>
       </c>
@@ -4231,7 +4565,7 @@
       <c r="F6" s="1"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="99"/>
+      <c r="A7" s="98"/>
       <c r="B7" s="2" t="s">
         <v>54</v>
       </c>
@@ -4243,7 +4577,7 @@
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" s="99"/>
+      <c r="A8" s="98"/>
       <c r="B8" s="38" t="s">
         <v>55</v>
       </c>
@@ -4255,7 +4589,7 @@
       <c r="F8" s="1"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9" s="99"/>
+      <c r="A9" s="98"/>
       <c r="B9" s="2" t="s">
         <v>56</v>
       </c>
@@ -4267,7 +4601,7 @@
       <c r="F9" s="1"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A10" s="99"/>
+      <c r="A10" s="98"/>
       <c r="B10" s="2" t="s">
         <v>57</v>
       </c>
@@ -4279,7 +4613,7 @@
       <c r="F10" s="1"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" s="99"/>
+      <c r="A11" s="98"/>
       <c r="B11" s="2" t="s">
         <v>58</v>
       </c>
@@ -4291,7 +4625,7 @@
       <c r="F11" s="1"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12" s="99"/>
+      <c r="A12" s="98"/>
       <c r="B12" s="2" t="s">
         <v>59</v>
       </c>
@@ -4303,7 +4637,7 @@
       <c r="F12" s="1"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A13" s="99"/>
+      <c r="A13" s="98"/>
       <c r="B13" s="2" t="s">
         <v>60</v>
       </c>
@@ -4315,7 +4649,7 @@
       <c r="F13" s="1"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A14" s="99"/>
+      <c r="A14" s="98"/>
       <c r="B14" s="38" t="s">
         <v>61</v>
       </c>
@@ -4327,7 +4661,7 @@
       <c r="F14" s="1"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A15" s="99"/>
+      <c r="A15" s="98"/>
       <c r="B15" s="38" t="s">
         <v>62</v>
       </c>
@@ -4339,7 +4673,7 @@
       <c r="F15" s="1"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A16" s="99"/>
+      <c r="A16" s="98"/>
       <c r="B16" s="41" t="s">
         <v>63</v>
       </c>
@@ -4351,7 +4685,7 @@
       <c r="F16" s="1"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A17" s="99"/>
+      <c r="A17" s="98"/>
       <c r="B17" s="38" t="s">
         <v>64</v>
       </c>
@@ -4363,7 +4697,7 @@
       <c r="F17" s="1"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A18" s="99"/>
+      <c r="A18" s="98"/>
       <c r="B18" s="41" t="s">
         <v>65</v>
       </c>
@@ -4375,7 +4709,7 @@
       <c r="F18" s="1"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A19" s="99"/>
+      <c r="A19" s="98"/>
       <c r="B19" s="38" t="s">
         <v>67</v>
       </c>
@@ -4387,7 +4721,7 @@
       <c r="F19" s="1"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A20" s="99"/>
+      <c r="A20" s="98"/>
       <c r="B20" s="38" t="s">
         <v>68</v>
       </c>
@@ -4399,7 +4733,7 @@
       <c r="F20" s="1"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A21" s="99"/>
+      <c r="A21" s="98"/>
       <c r="B21" s="38" t="s">
         <v>69</v>
       </c>
@@ -4411,7 +4745,7 @@
       <c r="F21" s="1"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A22" s="99"/>
+      <c r="A22" s="98"/>
       <c r="B22" s="38" t="s">
         <v>70</v>
       </c>
@@ -4423,7 +4757,7 @@
       <c r="F22" s="1"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A23" s="99"/>
+      <c r="A23" s="98"/>
       <c r="B23" s="38" t="s">
         <v>71</v>
       </c>
@@ -4435,7 +4769,7 @@
       <c r="F23" s="1"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A24" s="100"/>
+      <c r="A24" s="99"/>
       <c r="B24" s="38" t="s">
         <v>72</v>
       </c>
@@ -4455,7 +4789,7 @@
       <c r="F25" s="1"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A26" s="98" t="s">
+      <c r="A26" s="97" t="s">
         <v>36</v>
       </c>
       <c r="B26" s="2" t="s">
@@ -4468,7 +4802,7 @@
       <c r="F26" s="1"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A27" s="99"/>
+      <c r="A27" s="98"/>
       <c r="B27" s="2" t="s">
         <v>45</v>
       </c>
@@ -4480,7 +4814,7 @@
       <c r="F27" s="1"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A28" s="99"/>
+      <c r="A28" s="98"/>
       <c r="B28" s="2" t="s">
         <v>44</v>
       </c>
@@ -4492,7 +4826,7 @@
       <c r="F28" s="1"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A29" s="99"/>
+      <c r="A29" s="98"/>
       <c r="B29" s="2" t="s">
         <v>43</v>
       </c>
@@ -4504,7 +4838,7 @@
       <c r="F29" s="1"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A30" s="99"/>
+      <c r="A30" s="98"/>
       <c r="B30" s="2" t="s">
         <v>50</v>
       </c>
@@ -4516,7 +4850,7 @@
       <c r="F30" s="1"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A31" s="99"/>
+      <c r="A31" s="98"/>
       <c r="B31" s="2" t="s">
         <v>37</v>
       </c>
@@ -4528,7 +4862,7 @@
       <c r="F31" s="1"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A32" s="99"/>
+      <c r="A32" s="98"/>
       <c r="B32" s="2" t="s">
         <v>38</v>
       </c>
@@ -4540,7 +4874,7 @@
       <c r="F32" s="1"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A33" s="99"/>
+      <c r="A33" s="98"/>
       <c r="B33" s="2" t="s">
         <v>39</v>
       </c>
@@ -4552,7 +4886,7 @@
       <c r="F33" s="1"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A34" s="99"/>
+      <c r="A34" s="98"/>
       <c r="B34" s="26" t="s">
         <v>40</v>
       </c>
@@ -4564,7 +4898,7 @@
       <c r="F34" s="1"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A35" s="99"/>
+      <c r="A35" s="98"/>
       <c r="B35" s="2" t="s">
         <v>41</v>
       </c>
@@ -4576,7 +4910,7 @@
       <c r="F35" s="1"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A36" s="99"/>
+      <c r="A36" s="98"/>
       <c r="B36" s="2" t="s">
         <v>42</v>
       </c>
@@ -4588,7 +4922,7 @@
       <c r="F36" s="1"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A37" s="99"/>
+      <c r="A37" s="98"/>
       <c r="B37" s="2" t="s">
         <v>74</v>
       </c>
@@ -4608,10 +4942,10 @@
       <c r="F38" s="1"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A39" s="102" t="s">
+      <c r="A39" s="101" t="s">
         <v>31</v>
       </c>
-      <c r="B39" s="74" t="s">
+      <c r="B39" s="73" t="s">
         <v>32</v>
       </c>
       <c r="C39" s="25" t="s">
@@ -4621,7 +4955,7 @@
       <c r="E39" s="4"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A40" s="89"/>
+      <c r="A40" s="88"/>
       <c r="B40" s="17" t="s">
         <v>33</v>
       </c>
@@ -4632,7 +4966,7 @@
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A41" s="89"/>
+      <c r="A41" s="88"/>
       <c r="B41" s="17" t="s">
         <v>34</v>
       </c>
@@ -4644,7 +4978,7 @@
       <c r="H41" s="1"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A42" s="90"/>
+      <c r="A42" s="89"/>
       <c r="B42" s="17" t="s">
         <v>35</v>
       </c>
@@ -4662,7 +4996,7 @@
       <c r="E43" s="29"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A44" s="98" t="s">
+      <c r="A44" s="97" t="s">
         <v>13</v>
       </c>
       <c r="B44" s="2" t="s">
@@ -4675,7 +5009,7 @@
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A45" s="99"/>
+      <c r="A45" s="98"/>
       <c r="B45" s="2" t="s">
         <v>48</v>
       </c>
@@ -4686,7 +5020,7 @@
       </c>
     </row>
     <row r="46" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A46" s="101"/>
+      <c r="A46" s="100"/>
       <c r="B46" s="6" t="s">
         <v>49</v>
       </c>
@@ -4755,11 +5089,11 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A2" s="92" t="s">
+      <c r="A2" s="91" t="s">
         <v>79</v>
       </c>
-      <c r="B2" s="66" t="s">
-        <v>198</v>
+      <c r="B2" s="65" t="s">
+        <v>197</v>
       </c>
       <c r="C2" s="39"/>
       <c r="D2" s="40"/>
@@ -4769,9 +5103,9 @@
       <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A3" s="92"/>
-      <c r="B3" s="66" t="s">
-        <v>199</v>
+      <c r="A3" s="91"/>
+      <c r="B3" s="65" t="s">
+        <v>198</v>
       </c>
       <c r="C3" s="39"/>
       <c r="D3" s="40"/>
@@ -4781,9 +5115,9 @@
       <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A4" s="92"/>
-      <c r="B4" s="66" t="s">
-        <v>200</v>
+      <c r="A4" s="91"/>
+      <c r="B4" s="65" t="s">
+        <v>199</v>
       </c>
       <c r="C4" s="39"/>
       <c r="D4" s="40"/>
@@ -4793,9 +5127,9 @@
       <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" s="97"/>
-      <c r="B5" s="66" t="s">
-        <v>201</v>
+      <c r="A5" s="96"/>
+      <c r="B5" s="65" t="s">
+        <v>200</v>
       </c>
       <c r="C5" s="39"/>
       <c r="D5" s="40"/>
@@ -4813,11 +5147,11 @@
       <c r="F6" s="1"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A7" s="99" t="s">
-        <v>197</v>
+      <c r="A7" s="98" t="s">
+        <v>196</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
@@ -4827,9 +5161,9 @@
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A8" s="99"/>
+      <c r="A8" s="98"/>
       <c r="B8" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
@@ -4839,9 +5173,9 @@
       <c r="F8" s="1"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A9" s="99"/>
+      <c r="A9" s="98"/>
       <c r="B9" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
@@ -4851,9 +5185,9 @@
       <c r="F9" s="1"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A10" s="99"/>
+      <c r="A10" s="98"/>
       <c r="B10" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
@@ -4863,9 +5197,9 @@
       <c r="F10" s="1"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A11" s="99"/>
+      <c r="A11" s="98"/>
       <c r="B11" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
@@ -4875,9 +5209,9 @@
       <c r="F11" s="1"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A12" s="99"/>
+      <c r="A12" s="98"/>
       <c r="B12" s="26" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
@@ -4895,10 +5229,10 @@
       <c r="F13" s="1"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A14" s="102" t="s">
+      <c r="A14" s="101" t="s">
         <v>31</v>
       </c>
-      <c r="B14" s="74" t="s">
+      <c r="B14" s="73" t="s">
         <v>32</v>
       </c>
       <c r="C14" s="25" t="s">
@@ -4908,7 +5242,7 @@
       <c r="E14" s="4"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A15" s="89"/>
+      <c r="A15" s="88"/>
       <c r="B15" s="17" t="s">
         <v>34</v>
       </c>
@@ -4920,11 +5254,11 @@
       <c r="H15" s="1"/>
     </row>
     <row r="16" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="103"/>
-      <c r="B16" s="72" t="s">
+      <c r="A16" s="102"/>
+      <c r="B16" s="71" t="s">
         <v>35</v>
       </c>
-      <c r="C16" s="73" t="s">
+      <c r="C16" s="72" t="s">
         <v>12</v>
       </c>
       <c r="D16" s="6"/>
@@ -4959,7 +5293,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B77982FF-C4D2-41E8-A83F-1D743BC8CBAF}">
   <dimension ref="A1:E81"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A59" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="E77" sqref="E77"/>
     </sheetView>
   </sheetViews>
@@ -4987,7 +5321,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="94" t="s">
+      <c r="A2" s="93" t="s">
         <v>31</v>
       </c>
       <c r="B2" s="17" t="s">
@@ -5000,7 +5334,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="95"/>
+      <c r="A3" s="94"/>
       <c r="B3" s="17" t="s">
         <v>34</v>
       </c>
@@ -5011,7 +5345,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="95"/>
+      <c r="A4" s="94"/>
       <c r="B4" s="17" t="s">
         <v>35</v>
       </c>
@@ -5022,14 +5356,14 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="75"/>
+      <c r="A5" s="74"/>
       <c r="B5" s="55"/>
       <c r="C5" s="55"/>
       <c r="D5" s="55"/>
       <c r="E5" s="56"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="94" t="s">
+      <c r="A6" s="93" t="s">
         <v>76</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -5042,7 +5376,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="95"/>
+      <c r="A7" s="94"/>
       <c r="B7" s="52" t="s">
         <v>81</v>
       </c>
@@ -5053,7 +5387,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="95"/>
+      <c r="A8" s="94"/>
       <c r="B8" s="52" t="s">
         <v>92</v>
       </c>
@@ -5064,9 +5398,9 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="95"/>
-      <c r="B9" s="62" t="s">
-        <v>218</v>
+      <c r="A9" s="94"/>
+      <c r="B9" s="61" t="s">
+        <v>217</v>
       </c>
       <c r="C9" s="47"/>
       <c r="D9" s="53"/>
@@ -5075,8 +5409,8 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="95"/>
-      <c r="B10" s="62" t="s">
+      <c r="A10" s="94"/>
+      <c r="B10" s="61" t="s">
         <v>103</v>
       </c>
       <c r="C10" s="47"/>
@@ -5086,8 +5420,8 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="95"/>
-      <c r="B11" s="62" t="s">
+      <c r="A11" s="94"/>
+      <c r="B11" s="61" t="s">
         <v>104</v>
       </c>
       <c r="C11" s="47"/>
@@ -5097,8 +5431,8 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" s="95"/>
-      <c r="B12" s="62" t="s">
+      <c r="A12" s="94"/>
+      <c r="B12" s="61" t="s">
         <v>105</v>
       </c>
       <c r="C12" s="47"/>
@@ -5108,7 +5442,7 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" s="96"/>
+      <c r="A13" s="95"/>
       <c r="B13" s="54" t="s">
         <v>123</v>
       </c>
@@ -5126,7 +5460,7 @@
       <c r="E14" s="56"/>
     </row>
     <row r="15" spans="1:5" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="98" t="s">
+      <c r="A15" s="97" t="s">
         <v>78</v>
       </c>
       <c r="B15" s="2" t="s">
@@ -5139,9 +5473,9 @@
       </c>
     </row>
     <row r="16" spans="1:5" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="99"/>
+      <c r="A16" s="98"/>
       <c r="B16" s="17" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C16" s="47"/>
       <c r="D16" s="47"/>
@@ -5150,9 +5484,9 @@
       </c>
     </row>
     <row r="17" spans="1:5" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="99"/>
+      <c r="A17" s="98"/>
       <c r="B17" s="17" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C17" s="47"/>
       <c r="D17" s="47"/>
@@ -5161,9 +5495,9 @@
       </c>
     </row>
     <row r="18" spans="1:5" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="99"/>
+      <c r="A18" s="98"/>
       <c r="B18" s="17" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C18" s="47"/>
       <c r="D18" s="47"/>
@@ -5172,9 +5506,9 @@
       </c>
     </row>
     <row r="19" spans="1:5" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="99"/>
+      <c r="A19" s="98"/>
       <c r="B19" s="17" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C19" s="47"/>
       <c r="D19" s="47"/>
@@ -5183,9 +5517,9 @@
       </c>
     </row>
     <row r="20" spans="1:5" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="99"/>
+      <c r="A20" s="98"/>
       <c r="B20" s="17" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C20" s="47"/>
       <c r="D20" s="47"/>
@@ -5194,9 +5528,9 @@
       </c>
     </row>
     <row r="21" spans="1:5" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="99"/>
+      <c r="A21" s="98"/>
       <c r="B21" s="17" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C21" s="47"/>
       <c r="D21" s="47"/>
@@ -5205,9 +5539,9 @@
       </c>
     </row>
     <row r="22" spans="1:5" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="99"/>
+      <c r="A22" s="98"/>
       <c r="B22" s="17" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C22" s="47"/>
       <c r="D22" s="47"/>
@@ -5216,9 +5550,9 @@
       </c>
     </row>
     <row r="23" spans="1:5" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="99"/>
+      <c r="A23" s="98"/>
       <c r="B23" s="17" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C23" s="47"/>
       <c r="D23" s="47"/>
@@ -5227,9 +5561,9 @@
       </c>
     </row>
     <row r="24" spans="1:5" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="99"/>
+      <c r="A24" s="98"/>
       <c r="B24" s="17" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C24" s="47"/>
       <c r="D24" s="47"/>
@@ -5238,9 +5572,9 @@
       </c>
     </row>
     <row r="25" spans="1:5" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="99"/>
+      <c r="A25" s="98"/>
       <c r="B25" s="17" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C25" s="47"/>
       <c r="D25" s="47"/>
@@ -5249,9 +5583,9 @@
       </c>
     </row>
     <row r="26" spans="1:5" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="99"/>
+      <c r="A26" s="98"/>
       <c r="B26" s="17" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C26" s="47"/>
       <c r="D26" s="47"/>
@@ -5260,9 +5594,9 @@
       </c>
     </row>
     <row r="27" spans="1:5" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="99"/>
+      <c r="A27" s="98"/>
       <c r="B27" s="17" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C27" s="47"/>
       <c r="D27" s="47"/>
@@ -5271,9 +5605,9 @@
       </c>
     </row>
     <row r="28" spans="1:5" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="99"/>
+      <c r="A28" s="98"/>
       <c r="B28" s="17" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C28" s="47"/>
       <c r="D28" s="47"/>
@@ -5282,9 +5616,9 @@
       </c>
     </row>
     <row r="29" spans="1:5" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="99"/>
+      <c r="A29" s="98"/>
       <c r="B29" s="17" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C29" s="47"/>
       <c r="D29" s="47"/>
@@ -5293,9 +5627,9 @@
       </c>
     </row>
     <row r="30" spans="1:5" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="99"/>
+      <c r="A30" s="98"/>
       <c r="B30" s="17" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C30" s="47"/>
       <c r="D30" s="47"/>
@@ -5304,9 +5638,9 @@
       </c>
     </row>
     <row r="31" spans="1:5" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="99"/>
+      <c r="A31" s="98"/>
       <c r="B31" s="17" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C31" s="47"/>
       <c r="D31" s="47"/>
@@ -5315,9 +5649,9 @@
       </c>
     </row>
     <row r="32" spans="1:5" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="99"/>
+      <c r="A32" s="98"/>
       <c r="B32" s="17" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C32" s="47"/>
       <c r="D32" s="47"/>
@@ -5326,9 +5660,9 @@
       </c>
     </row>
     <row r="33" spans="1:5" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="99"/>
+      <c r="A33" s="98"/>
       <c r="B33" s="17" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C33" s="47"/>
       <c r="D33" s="47"/>
@@ -5337,9 +5671,9 @@
       </c>
     </row>
     <row r="34" spans="1:5" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="99"/>
+      <c r="A34" s="98"/>
       <c r="B34" s="17" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C34" s="47"/>
       <c r="D34" s="47"/>
@@ -5348,9 +5682,9 @@
       </c>
     </row>
     <row r="35" spans="1:5" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="99"/>
+      <c r="A35" s="98"/>
       <c r="B35" s="17" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C35" s="47"/>
       <c r="D35" s="47"/>
@@ -5359,16 +5693,16 @@
       </c>
     </row>
     <row r="36" spans="1:5" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="99"/>
+      <c r="A36" s="98"/>
       <c r="B36" s="17"/>
       <c r="C36" s="47"/>
       <c r="D36" s="47"/>
       <c r="E36" s="31"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A37" s="99"/>
+      <c r="A37" s="98"/>
       <c r="B37" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C37" s="47"/>
       <c r="D37" s="47"/>
@@ -5377,9 +5711,9 @@
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A38" s="99"/>
+      <c r="A38" s="98"/>
       <c r="B38" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C38" s="47"/>
       <c r="D38" s="47"/>
@@ -5388,9 +5722,9 @@
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A39" s="99"/>
+      <c r="A39" s="98"/>
       <c r="B39" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C39" s="47"/>
       <c r="D39" s="47"/>
@@ -5399,9 +5733,9 @@
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A40" s="99"/>
+      <c r="A40" s="98"/>
       <c r="B40" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C40" s="47"/>
       <c r="D40" s="47"/>
@@ -5410,9 +5744,9 @@
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A41" s="99"/>
+      <c r="A41" s="98"/>
       <c r="B41" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C41" s="47"/>
       <c r="D41" s="47"/>
@@ -5421,9 +5755,9 @@
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A42" s="99"/>
+      <c r="A42" s="98"/>
       <c r="B42" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C42" s="47"/>
       <c r="D42" s="47"/>
@@ -5432,9 +5766,9 @@
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A43" s="99"/>
+      <c r="A43" s="98"/>
       <c r="B43" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C43" s="47"/>
       <c r="D43" s="47"/>
@@ -5443,9 +5777,9 @@
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A44" s="99"/>
+      <c r="A44" s="98"/>
       <c r="B44" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C44" s="47"/>
       <c r="D44" s="47"/>
@@ -5454,9 +5788,9 @@
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A45" s="99"/>
+      <c r="A45" s="98"/>
       <c r="B45" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C45" s="47"/>
       <c r="D45" s="47"/>
@@ -5465,9 +5799,9 @@
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A46" s="99"/>
+      <c r="A46" s="98"/>
       <c r="B46" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C46" s="47"/>
       <c r="D46" s="47"/>
@@ -5476,9 +5810,9 @@
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A47" s="99"/>
+      <c r="A47" s="98"/>
       <c r="B47" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C47" s="47"/>
       <c r="D47" s="47"/>
@@ -5487,9 +5821,9 @@
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A48" s="99"/>
+      <c r="A48" s="98"/>
       <c r="B48" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C48" s="47"/>
       <c r="D48" s="47"/>
@@ -5498,9 +5832,9 @@
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A49" s="99"/>
+      <c r="A49" s="98"/>
       <c r="B49" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C49" s="47"/>
       <c r="D49" s="47"/>
@@ -5509,9 +5843,9 @@
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A50" s="99"/>
+      <c r="A50" s="98"/>
       <c r="B50" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C50" s="47"/>
       <c r="D50" s="47"/>
@@ -5520,9 +5854,9 @@
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A51" s="99"/>
+      <c r="A51" s="98"/>
       <c r="B51" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C51" s="47"/>
       <c r="D51" s="47"/>
@@ -5531,9 +5865,9 @@
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A52" s="99"/>
+      <c r="A52" s="98"/>
       <c r="B52" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C52" s="47"/>
       <c r="D52" s="47"/>
@@ -5542,9 +5876,9 @@
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A53" s="99"/>
+      <c r="A53" s="98"/>
       <c r="B53" s="26" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C53" s="47"/>
       <c r="D53" s="47"/>
@@ -5553,9 +5887,9 @@
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A54" s="99"/>
+      <c r="A54" s="98"/>
       <c r="B54" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C54" s="47"/>
       <c r="D54" s="47"/>
@@ -5564,9 +5898,9 @@
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A55" s="99"/>
+      <c r="A55" s="98"/>
       <c r="B55" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C55" s="47"/>
       <c r="D55" s="47"/>
@@ -5575,9 +5909,9 @@
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A56" s="99"/>
+      <c r="A56" s="98"/>
       <c r="B56" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C56" s="47"/>
       <c r="D56" s="47"/>
@@ -5586,14 +5920,14 @@
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A57" s="75"/>
+      <c r="A57" s="74"/>
       <c r="B57" s="55"/>
       <c r="C57" s="55"/>
       <c r="D57" s="55"/>
       <c r="E57" s="56"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A58" s="98" t="s">
+      <c r="A58" s="97" t="s">
         <v>79</v>
       </c>
       <c r="B58" s="17" t="s">
@@ -5606,7 +5940,7 @@
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A59" s="99"/>
+      <c r="A59" s="98"/>
       <c r="B59" s="17" t="s">
         <v>94</v>
       </c>
@@ -5617,7 +5951,7 @@
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A60" s="100"/>
+      <c r="A60" s="99"/>
       <c r="B60" s="17" t="s">
         <v>93</v>
       </c>
@@ -5628,14 +5962,14 @@
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A61" s="75"/>
+      <c r="A61" s="74"/>
       <c r="B61" s="55"/>
       <c r="C61" s="55"/>
       <c r="D61" s="55"/>
       <c r="E61" s="55"/>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A62" s="94" t="s">
+      <c r="A62" s="93" t="s">
         <v>82</v>
       </c>
       <c r="B62" s="2" t="s">
@@ -5648,7 +5982,7 @@
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A63" s="95"/>
+      <c r="A63" s="94"/>
       <c r="B63" s="2" t="s">
         <v>84</v>
       </c>
@@ -5659,7 +5993,7 @@
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A64" s="95"/>
+      <c r="A64" s="94"/>
       <c r="B64" s="2" t="s">
         <v>87</v>
       </c>
@@ -5670,7 +6004,7 @@
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A65" s="95"/>
+      <c r="A65" s="94"/>
       <c r="B65" s="2" t="s">
         <v>85</v>
       </c>
@@ -5681,7 +6015,7 @@
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A66" s="95"/>
+      <c r="A66" s="94"/>
       <c r="B66" s="2" t="s">
         <v>86</v>
       </c>
@@ -5692,152 +6026,152 @@
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A67" s="95"/>
-      <c r="B67" s="58" t="s">
+      <c r="A67" s="94"/>
+      <c r="B67" s="57" t="s">
         <v>88</v>
       </c>
       <c r="C67" s="25"/>
-      <c r="D67" s="59"/>
+      <c r="D67" s="58"/>
       <c r="E67" s="31" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A68" s="95"/>
-      <c r="B68" s="58" t="s">
+      <c r="A68" s="94"/>
+      <c r="B68" s="57" t="s">
         <v>89</v>
       </c>
       <c r="C68" s="25"/>
-      <c r="D68" s="59"/>
+      <c r="D68" s="58"/>
       <c r="E68" s="31" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A69" s="95"/>
-      <c r="B69" s="58" t="s">
+      <c r="A69" s="94"/>
+      <c r="B69" s="57" t="s">
         <v>90</v>
       </c>
       <c r="C69" s="25"/>
-      <c r="D69" s="59"/>
-      <c r="E69" s="60" t="s">
+      <c r="D69" s="58"/>
+      <c r="E69" s="59" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A70" s="95"/>
-      <c r="B70" s="61" t="s">
+      <c r="A70" s="94"/>
+      <c r="B70" s="60" t="s">
         <v>91</v>
       </c>
       <c r="C70" s="25"/>
-      <c r="D70" s="59"/>
-      <c r="E70" s="71" t="s">
+      <c r="D70" s="58"/>
+      <c r="E70" s="70" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A71" s="96"/>
-      <c r="B71" s="61" t="s">
-        <v>159</v>
+      <c r="A71" s="95"/>
+      <c r="B71" s="60" t="s">
+        <v>158</v>
       </c>
       <c r="C71" s="25"/>
-      <c r="D71" s="59"/>
-      <c r="E71" s="71" t="s">
+      <c r="D71" s="58"/>
+      <c r="E71" s="70" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A72" s="75"/>
+      <c r="A72" s="74"/>
       <c r="B72" s="55"/>
       <c r="C72" s="55"/>
       <c r="D72" s="55"/>
-      <c r="E72" s="63"/>
+      <c r="E72" s="62"/>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A73" s="94" t="s">
+      <c r="A73" s="93" t="s">
         <v>96</v>
       </c>
-      <c r="B73" s="61" t="s">
-        <v>219</v>
-      </c>
-      <c r="C73" s="64"/>
-      <c r="D73" s="59"/>
-      <c r="E73" s="60" t="s">
+      <c r="B73" s="60" t="s">
+        <v>218</v>
+      </c>
+      <c r="C73" s="63"/>
+      <c r="D73" s="58"/>
+      <c r="E73" s="59" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A74" s="95"/>
-      <c r="B74" s="61" t="s">
+      <c r="A74" s="94"/>
+      <c r="B74" s="60" t="s">
         <v>95</v>
       </c>
-      <c r="C74" s="64" t="s">
-        <v>12</v>
-      </c>
-      <c r="D74" s="59"/>
-      <c r="E74" s="60"/>
+      <c r="C74" s="63" t="s">
+        <v>12</v>
+      </c>
+      <c r="D74" s="58"/>
+      <c r="E74" s="59"/>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A75" s="95"/>
-      <c r="B75" s="61" t="s">
+      <c r="A75" s="94"/>
+      <c r="B75" s="60" t="s">
         <v>97</v>
       </c>
-      <c r="C75" s="64" t="s">
-        <v>12</v>
-      </c>
-      <c r="D75" s="59"/>
-      <c r="E75" s="60"/>
+      <c r="C75" s="63" t="s">
+        <v>12</v>
+      </c>
+      <c r="D75" s="58"/>
+      <c r="E75" s="59"/>
     </row>
     <row r="76" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A76" s="95"/>
-      <c r="B76" s="61" t="s">
+      <c r="A76" s="94"/>
+      <c r="B76" s="60" t="s">
         <v>98</v>
       </c>
-      <c r="C76" s="64" t="s">
-        <v>12</v>
-      </c>
-      <c r="D76" s="59"/>
-      <c r="E76" s="60"/>
+      <c r="C76" s="63" t="s">
+        <v>12</v>
+      </c>
+      <c r="D76" s="58"/>
+      <c r="E76" s="59"/>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A77" s="95"/>
-      <c r="B77" s="61" t="s">
+      <c r="A77" s="94"/>
+      <c r="B77" s="60" t="s">
         <v>102</v>
       </c>
-      <c r="C77" s="64" t="s">
-        <v>12</v>
-      </c>
-      <c r="D77" s="59"/>
-      <c r="E77" s="60"/>
+      <c r="C77" s="63" t="s">
+        <v>12</v>
+      </c>
+      <c r="D77" s="58"/>
+      <c r="E77" s="59"/>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A78" s="95"/>
-      <c r="B78" s="61" t="s">
+      <c r="A78" s="94"/>
+      <c r="B78" s="60" t="s">
         <v>99</v>
       </c>
-      <c r="C78" s="64" t="s">
-        <v>12</v>
-      </c>
-      <c r="D78" s="59"/>
-      <c r="E78" s="60"/>
+      <c r="C78" s="63" t="s">
+        <v>12</v>
+      </c>
+      <c r="D78" s="58"/>
+      <c r="E78" s="59"/>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A79" s="95"/>
-      <c r="B79" s="61" t="s">
+      <c r="A79" s="94"/>
+      <c r="B79" s="60" t="s">
         <v>100</v>
       </c>
-      <c r="C79" s="64" t="s">
-        <v>12</v>
-      </c>
-      <c r="D79" s="59"/>
-      <c r="E79" s="60"/>
+      <c r="C79" s="63" t="s">
+        <v>12</v>
+      </c>
+      <c r="D79" s="58"/>
+      <c r="E79" s="59"/>
     </row>
     <row r="80" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A80" s="104"/>
-      <c r="B80" s="72" t="s">
+      <c r="A80" s="103"/>
+      <c r="B80" s="71" t="s">
         <v>101</v>
       </c>
-      <c r="C80" s="73" t="s">
+      <c r="C80" s="72" t="s">
         <v>12</v>
       </c>
       <c r="D80" s="48"/>
@@ -5866,16 +6200,16 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACF97C5A-E76A-4F7F-AE1B-EEE4815545E3}">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:E17"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="19.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="47.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="79.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
@@ -5896,10 +6230,12 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="57" t="s">
-        <v>125</v>
-      </c>
-      <c r="B2" s="2"/>
+      <c r="A2" s="104" t="s">
+        <v>229</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>230</v>
+      </c>
       <c r="C2" s="47" t="s">
         <v>12</v>
       </c>
@@ -5908,18 +6244,22 @@
       <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="82"/>
-      <c r="B3" s="84"/>
-      <c r="C3" s="84"/>
-      <c r="D3" s="84"/>
-      <c r="E3" s="85"/>
+      <c r="A3" s="105"/>
+      <c r="B3" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="C3" s="47" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="4"/>
       <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="B4" s="2"/>
+      <c r="A4" s="105"/>
+      <c r="B4" s="2" t="s">
+        <v>232</v>
+      </c>
       <c r="C4" s="47" t="s">
         <v>12</v>
       </c>
@@ -5929,181 +6269,415 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="105"/>
-      <c r="B5" s="83"/>
-      <c r="C5" s="83"/>
-      <c r="D5" s="84"/>
-      <c r="E5" s="85"/>
+      <c r="B5" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="C5" s="47" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="4"/>
       <c r="F5" s="1"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="95" t="s">
-        <v>96</v>
-      </c>
-      <c r="B6" s="61" t="s">
-        <v>95</v>
-      </c>
-      <c r="C6" s="64" t="s">
+      <c r="A6" s="105"/>
+      <c r="B6" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="C6" s="47" t="s">
         <v>12</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="4"/>
+      <c r="F6" s="1"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="95"/>
-      <c r="B7" s="61" t="s">
-        <v>97</v>
-      </c>
-      <c r="C7" s="64" t="s">
+      <c r="A7" s="105"/>
+      <c r="B7" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="C7" s="47" t="s">
         <v>12</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="4"/>
-    </row>
-    <row r="8" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="95"/>
-      <c r="B8" s="61" t="s">
-        <v>98</v>
-      </c>
-      <c r="C8" s="64" t="s">
+      <c r="F7" s="1"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" s="105"/>
+      <c r="B8" s="17" t="s">
+        <v>236</v>
+      </c>
+      <c r="C8" s="47" t="s">
         <v>12</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="4"/>
+      <c r="F8" s="1"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9" s="95"/>
-      <c r="B9" s="61" t="s">
-        <v>102</v>
-      </c>
-      <c r="C9" s="64" t="s">
+      <c r="A9" s="105"/>
+      <c r="B9" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="C9" s="47" t="s">
         <v>12</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="4"/>
+      <c r="F9" s="1"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A10" s="95"/>
-      <c r="B10" s="61" t="s">
-        <v>99</v>
-      </c>
-      <c r="C10" s="64" t="s">
+      <c r="A10" s="105"/>
+      <c r="B10" s="26" t="s">
+        <v>238</v>
+      </c>
+      <c r="C10" s="47" t="s">
         <v>12</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="4"/>
+      <c r="F10" s="1"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" s="95"/>
-      <c r="B11" s="61" t="s">
-        <v>100</v>
-      </c>
-      <c r="C11" s="64" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11" s="2"/>
-      <c r="E11" s="4"/>
+      <c r="A11" s="105"/>
+      <c r="B11" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="C11" s="47" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="38"/>
+      <c r="E11" s="107"/>
+      <c r="F11" s="1"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12" s="96"/>
-      <c r="B12" s="17" t="s">
-        <v>101</v>
-      </c>
-      <c r="C12" s="25" t="s">
-        <v>12</v>
-      </c>
-      <c r="D12" s="2"/>
-      <c r="E12" s="4"/>
+      <c r="A12" s="106"/>
+      <c r="B12" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="C12" s="47" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="38"/>
+      <c r="E12" s="107"/>
+      <c r="F12" s="1"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A13" s="86"/>
-      <c r="B13" s="87"/>
-      <c r="C13" s="87"/>
-      <c r="D13" s="84"/>
-      <c r="E13" s="85"/>
+      <c r="A13" s="81"/>
+      <c r="B13" s="81"/>
+      <c r="C13" s="81"/>
+      <c r="D13" s="81"/>
+      <c r="E13" s="81"/>
+      <c r="F13" s="1"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A14" s="94" t="s">
-        <v>76</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="C14" s="25" t="s">
+      <c r="A14" s="104" t="s">
+        <v>222</v>
+      </c>
+      <c r="B14" s="57" t="s">
+        <v>223</v>
+      </c>
+      <c r="C14" s="63" t="s">
         <v>12</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="4"/>
+      <c r="F14" s="1"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A15" s="95"/>
-      <c r="B15" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="C15" s="25" t="s">
+      <c r="A15" s="105"/>
+      <c r="B15" s="57" t="s">
+        <v>224</v>
+      </c>
+      <c r="C15" s="63" t="s">
         <v>12</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="4"/>
+      <c r="F15" s="1"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A16" s="96"/>
-      <c r="B16" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="C16" s="25" t="s">
+      <c r="A16" s="105"/>
+      <c r="B16" s="57" t="s">
+        <v>225</v>
+      </c>
+      <c r="C16" s="63" t="s">
         <v>12</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="4"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17" s="105"/>
-      <c r="B17" s="84"/>
-      <c r="C17" s="84"/>
-      <c r="D17" s="84"/>
-      <c r="E17" s="85"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A18" s="3"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="4"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A19" s="3"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
+      <c r="F16" s="1"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17" s="106"/>
+      <c r="B17" s="57" t="s">
+        <v>226</v>
+      </c>
+      <c r="C17" s="63" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" s="2"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="1"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18" s="86"/>
+      <c r="B18" s="81"/>
+      <c r="C18" s="81"/>
+      <c r="D18" s="82"/>
+      <c r="E18" s="83"/>
+      <c r="F18" s="1"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19" s="94" t="s">
+        <v>96</v>
+      </c>
+      <c r="B19" s="60" t="s">
+        <v>95</v>
+      </c>
+      <c r="C19" s="63" t="s">
+        <v>12</v>
+      </c>
       <c r="D19" s="2"/>
       <c r="E19" s="4"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A20" s="3"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A20" s="94"/>
+      <c r="B20" s="60" t="s">
+        <v>97</v>
+      </c>
+      <c r="C20" s="63" t="s">
+        <v>12</v>
+      </c>
       <c r="D20" s="2"/>
       <c r="E20" s="4"/>
     </row>
-    <row r="21" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="5"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="7"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
+    <row r="21" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A21" s="94"/>
+      <c r="B21" s="60" t="s">
+        <v>98</v>
+      </c>
+      <c r="C21" s="63" t="s">
+        <v>12</v>
+      </c>
+      <c r="D21" s="2"/>
+      <c r="E21" s="4"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A22" s="94"/>
+      <c r="B22" s="60" t="s">
+        <v>102</v>
+      </c>
+      <c r="C22" s="63" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22" s="2"/>
+      <c r="E22" s="4"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A23" s="94"/>
+      <c r="B23" s="60" t="s">
+        <v>99</v>
+      </c>
+      <c r="C23" s="63" t="s">
+        <v>12</v>
+      </c>
+      <c r="D23" s="2"/>
+      <c r="E23" s="4"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A24" s="94"/>
+      <c r="B24" s="60" t="s">
+        <v>100</v>
+      </c>
+      <c r="C24" s="63" t="s">
+        <v>12</v>
+      </c>
+      <c r="D24" s="2"/>
+      <c r="E24" s="4"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A25" s="95"/>
+      <c r="B25" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="C25" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="D25" s="2"/>
+      <c r="E25" s="4"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A26" s="84"/>
+      <c r="B26" s="85"/>
+      <c r="C26" s="85"/>
+      <c r="D26" s="82"/>
+      <c r="E26" s="83"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A27" s="93" t="s">
+        <v>76</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="C27" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="D27" s="2"/>
+      <c r="E27" s="4"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A28" s="94"/>
+      <c r="B28" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="C28" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="D28" s="2"/>
+      <c r="E28" s="4"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A29" s="95"/>
+      <c r="B29" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="C29" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="D29" s="2"/>
+      <c r="E29" s="4"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A30" s="86"/>
+      <c r="B30" s="82"/>
+      <c r="C30" s="82"/>
+      <c r="D30" s="82"/>
+      <c r="E30" s="83"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A31" s="3"/>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="4"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A32" s="3"/>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="4"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A33" s="3"/>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="4"/>
+    </row>
+    <row r="34" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A34" s="5"/>
+      <c r="B34" s="6"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="7"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A35" s="1"/>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A6:A12"/>
-    <mergeCell ref="A14:A16"/>
+  <mergeCells count="4">
+    <mergeCell ref="A19:A25"/>
+    <mergeCell ref="A27:A29"/>
+    <mergeCell ref="A14:A17"/>
+    <mergeCell ref="A2:A12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0A365AE-7930-4274-837C-B5D83DFDF1FE}">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="18.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="44" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="45" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="45" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="45" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="46" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="47" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="4"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="3"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="47" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="38"/>
+      <c r="E3" s="107"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="3"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="47" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="4"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="38"/>
+      <c r="B5" s="38"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="4"/>
+    </row>
+    <row r="6" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>